<commit_message>
Add Pontiki and contacts page
</commit_message>
<xml_diff>
--- a/Somewhere Census.xlsx
+++ b/Somewhere Census.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\campaigns\fractured-worlds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBA43C7-B4D1-4823-BFC1-9A2F2185176F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0AE7FD-4908-4761-8CF9-C95B37CBB334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{206A7769-913C-44FD-A917-4F208E1EA77B}"/>
   </bookViews>
@@ -661,9 +661,6 @@
     <t>Employees #</t>
   </si>
   <si>
-    <t>Deldrig Helcral</t>
-  </si>
-  <si>
     <t>Saélihn Mason</t>
   </si>
   <si>
@@ -998,6 +995,9 @@
   </si>
   <si>
     <t>Ageless</t>
+  </si>
+  <si>
+    <t>Deldric Helcral</t>
   </si>
 </sst>
 </file>
@@ -1938,10 +1938,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>100</v>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B2" s="29">
         <f>B4-B3</f>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B3" s="29">
         <f>COUNTIF(Citizens[Is Permanent Resident?],FALSE)</f>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B4" s="29">
         <f>COUNTIF(Citizens[Arrived],TRUE)</f>
@@ -2000,10 +2000,10 @@
   <dimension ref="A1:U79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="H52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W66" sqref="W66"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,7 +2126,7 @@
         <v>13</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P3" s="24" t="s">
         <v>14</v>
@@ -2138,10 +2138,10 @@
         <v>18</v>
       </c>
       <c r="S3" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="T3" s="21" t="s">
         <v>277</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>278</v>
       </c>
       <c r="U3" s="23" t="s">
         <v>15</v>
@@ -2149,7 +2149,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
@@ -2159,7 +2159,7 @@
         <v>97</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>93</v>
@@ -2178,10 +2178,10 @@
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O4" s="26" t="s">
         <v>86</v>
@@ -2197,7 +2197,7 @@
         <v>36990</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T4" s="9" t="b">
         <v>1</v>
@@ -2255,7 +2255,7 @@
         <v>36941</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T5" s="7" t="b">
         <v>1</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" t="s">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="I6" s="18"/>
       <c r="M6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N6" t="s">
         <v>196</v>
@@ -2300,13 +2300,13 @@
         <v>36988</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T6" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2358,13 +2358,13 @@
         <v>36951</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2410,13 +2410,13 @@
         <v>36951</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T8" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
         <v>36989</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T9" s="7" t="b">
         <v>1</v>
@@ -2511,7 +2511,7 @@
         <v>36934</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T10" s="7" t="b">
         <v>1</v>
@@ -2559,7 +2559,7 @@
         <v>36984</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T11" s="7" t="b">
         <v>1</v>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="I12" s="18"/>
       <c r="M12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N12" t="s">
         <v>56</v>
@@ -2607,7 +2607,7 @@
         <v>36934</v>
       </c>
       <c r="S12" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T12" s="7" t="b">
         <v>1</v>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" t="s">
@@ -2626,7 +2626,7 @@
         <v>97</v>
       </c>
       <c r="F13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>98</v>
@@ -2635,7 +2635,7 @@
         <v>45499</v>
       </c>
       <c r="M13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N13" t="s">
         <v>193</v>
@@ -2654,7 +2654,7 @@
         <v>36989</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T13" s="7" t="b">
         <v>1</v>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="I14" s="18"/>
       <c r="M14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N14" t="s">
         <v>188</v>
@@ -2698,13 +2698,13 @@
         <v>36919</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T14" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2754,13 +2754,13 @@
         <v>36951</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T15" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -2801,13 +2801,13 @@
         <v>36986</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T16" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -2819,7 +2819,7 @@
         <v>110</v>
       </c>
       <c r="E17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F17" t="s">
         <v>138</v>
@@ -2851,7 +2851,7 @@
         <v>36971</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T17" s="7" t="b">
         <v>1</v>
@@ -2905,7 +2905,7 @@
         <v>36927</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T18" s="7" t="b">
         <v>1</v>
@@ -2914,7 +2914,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" t="s">
@@ -2931,7 +2931,7 @@
       </c>
       <c r="I19" s="18"/>
       <c r="M19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N19" t="s">
         <v>194</v>
@@ -2950,18 +2950,18 @@
         <v>36988</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T19" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U19" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" t="s">
@@ -2977,13 +2977,13 @@
         <v>98</v>
       </c>
       <c r="H20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I20" s="18">
         <v>45598</v>
       </c>
       <c r="M20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N20" t="s">
         <v>77</v>
@@ -3002,7 +3002,7 @@
         <v>36987</v>
       </c>
       <c r="S20" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T20" s="7" t="b">
         <v>1</v>
@@ -3013,14 +3013,14 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>198</v>
+        <v>310</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" t="s">
         <v>110</v>
       </c>
       <c r="E21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>142</v>
@@ -3049,7 +3049,7 @@
         <v>36949</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T21" s="7" t="b">
         <v>1</v>
@@ -3058,10 +3058,10 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D22" t="s">
         <v>111</v>
@@ -3070,7 +3070,7 @@
         <v>132</v>
       </c>
       <c r="F22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>142</v>
@@ -3086,7 +3086,7 @@
         <v>160</v>
       </c>
       <c r="M22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N22" t="s">
         <v>81</v>
@@ -3105,7 +3105,7 @@
         <v>36993</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T22" s="7" t="b">
         <v>1</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" t="s">
@@ -3131,7 +3131,7 @@
       </c>
       <c r="I23" s="18"/>
       <c r="M23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N23" t="s">
         <v>195</v>
@@ -3150,7 +3150,7 @@
         <v>36966</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T23" s="7" t="b">
         <v>1</v>
@@ -3204,7 +3204,7 @@
         <v>36983</v>
       </c>
       <c r="S24" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="T24" s="7" t="b">
         <v>1</v>
@@ -3258,7 +3258,7 @@
         <v>36927</v>
       </c>
       <c r="S25" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T25" s="7" t="b">
         <v>1</v>
@@ -3300,7 +3300,7 @@
         <v>36987</v>
       </c>
       <c r="S26" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T26" s="7" t="b">
         <v>1</v>
@@ -3350,7 +3350,7 @@
         <v>36982</v>
       </c>
       <c r="S27" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T27" s="7" t="b">
         <v>1</v>
@@ -3366,7 +3366,7 @@
         <v>110</v>
       </c>
       <c r="E28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>93</v>
@@ -3384,13 +3384,13 @@
         <v>36986</v>
       </c>
       <c r="S28" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T28" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U28" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -3431,7 +3431,7 @@
         <v>36986</v>
       </c>
       <c r="S29" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T29" s="7" t="b">
         <v>1</v>
@@ -3470,7 +3470,7 @@
         <v>160</v>
       </c>
       <c r="M30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N30" t="s">
         <v>39</v>
@@ -3489,7 +3489,7 @@
         <v>36959</v>
       </c>
       <c r="S30" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T30" s="7" t="b">
         <v>1</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" t="s">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="I31" s="18"/>
       <c r="M31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N31" t="s">
         <v>59</v>
@@ -3537,7 +3537,7 @@
         <v>36991</v>
       </c>
       <c r="S31" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T31" s="7" t="b">
         <v>1</v>
@@ -3579,7 +3579,7 @@
         <v>36989</v>
       </c>
       <c r="S32" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T32" s="7" t="b">
         <v>1</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" t="s">
@@ -3600,7 +3600,7 @@
         <v>115</v>
       </c>
       <c r="F33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>142</v>
@@ -3635,18 +3635,18 @@
         <v>36993</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T33" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U33" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" t="s">
@@ -3656,7 +3656,7 @@
         <v>97</v>
       </c>
       <c r="F34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>98</v>
@@ -3665,10 +3665,10 @@
         <v>31052</v>
       </c>
       <c r="M34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N34" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>165</v>
@@ -3684,7 +3684,7 @@
         <v>36989</v>
       </c>
       <c r="S34" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T34" s="7" t="b">
         <v>1</v>
@@ -3737,13 +3737,13 @@
         <v>36986</v>
       </c>
       <c r="S35" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T35" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U35" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -3768,7 +3768,7 @@
       </c>
       <c r="I36" s="18"/>
       <c r="M36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N36" t="s">
         <v>75</v>
@@ -3785,13 +3785,13 @@
         <v>36986</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T36" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U36" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3817,7 +3817,7 @@
       <c r="I37" s="18"/>
       <c r="J37" s="5"/>
       <c r="M37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N37" t="s">
         <v>188</v>
@@ -3836,13 +3836,13 @@
         <v>36986</v>
       </c>
       <c r="S37" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T37" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -3855,7 +3855,7 @@
         <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>98</v>
@@ -3863,7 +3863,7 @@
       <c r="I38" s="18"/>
       <c r="J38" s="5"/>
       <c r="M38" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N38" t="s">
         <v>66</v>
@@ -3880,18 +3880,18 @@
         <v>36986</v>
       </c>
       <c r="S38" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T38" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="5" t="s">
@@ -3920,7 +3920,7 @@
         <v>143</v>
       </c>
       <c r="M39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N39" t="s">
         <v>79</v>
@@ -3939,7 +3939,7 @@
         <v>36967</v>
       </c>
       <c r="S39" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T39" s="7" t="b">
         <v>1</v>
@@ -3980,18 +3980,18 @@
         <v>36916</v>
       </c>
       <c r="S40" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T40" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
@@ -4002,7 +4002,7 @@
         <v>115</v>
       </c>
       <c r="F41" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>142</v>
@@ -4010,7 +4010,7 @@
       <c r="I41" s="18"/>
       <c r="J41" s="5"/>
       <c r="M41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N41" t="s">
         <v>65</v>
@@ -4026,13 +4026,13 @@
         <v>36978</v>
       </c>
       <c r="S41" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T41" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -4066,7 +4066,7 @@
         <v>143</v>
       </c>
       <c r="M42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N42" t="s">
         <v>43</v>
@@ -4085,13 +4085,13 @@
         <v>36951</v>
       </c>
       <c r="S42" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T42" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
@@ -4137,7 +4137,7 @@
         <v>36950</v>
       </c>
       <c r="S43" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T43" s="7" t="b">
         <v>1</v>
@@ -4191,7 +4191,7 @@
         <v>36953</v>
       </c>
       <c r="S44" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T44" s="7" t="b">
         <v>1</v>
@@ -4199,11 +4199,11 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D45" t="s">
         <v>111</v>
@@ -4212,7 +4212,7 @@
         <v>128</v>
       </c>
       <c r="F45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>162</v>
@@ -4223,7 +4223,7 @@
       <c r="I45" s="18"/>
       <c r="J45" s="5"/>
       <c r="M45" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N45" t="s">
         <v>81</v>
@@ -4242,7 +4242,7 @@
         <v>36992</v>
       </c>
       <c r="S45" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T45" s="7" t="b">
         <v>1</v>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="5"/>
@@ -4288,7 +4288,7 @@
         <v>36987</v>
       </c>
       <c r="S46" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T46" s="7" t="b">
         <v>1</v>
@@ -4299,7 +4299,7 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="5"/>
@@ -4318,7 +4318,7 @@
       <c r="I47" s="18"/>
       <c r="J47" s="5"/>
       <c r="M47" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N47" t="s">
         <v>194</v>
@@ -4337,18 +4337,18 @@
         <v>36988</v>
       </c>
       <c r="S47" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T47" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U47" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
@@ -4359,7 +4359,7 @@
         <v>97</v>
       </c>
       <c r="F48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>93</v>
@@ -4383,7 +4383,7 @@
         <v>36989</v>
       </c>
       <c r="S48" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T48" s="7" t="b">
         <v>1</v>
@@ -4402,7 +4402,7 @@
         <v>110</v>
       </c>
       <c r="E49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>98</v>
@@ -4410,7 +4410,7 @@
       <c r="I49" s="18"/>
       <c r="J49" s="5"/>
       <c r="M49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N49" t="s">
         <v>66</v>
@@ -4427,18 +4427,18 @@
         <v>36986</v>
       </c>
       <c r="S49" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T49" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="5"/>
@@ -4449,7 +4449,7 @@
         <v>97</v>
       </c>
       <c r="F50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>93</v>
@@ -4473,7 +4473,7 @@
         <v>36989</v>
       </c>
       <c r="S50" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T50" s="7" t="b">
         <v>1</v>
@@ -4532,7 +4532,7 @@
         <v>36969</v>
       </c>
       <c r="S51" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T51" s="7" t="b">
         <v>1</v>
@@ -4581,7 +4581,7 @@
         <v>36927</v>
       </c>
       <c r="S52" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T52" s="7" t="b">
         <v>1</v>
@@ -4611,7 +4611,7 @@
       <c r="I53" s="18"/>
       <c r="J53" s="5"/>
       <c r="M53" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N53" t="s">
         <v>69</v>
@@ -4630,18 +4630,18 @@
         <v>36986</v>
       </c>
       <c r="S53" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T53" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U53" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="5"/>
@@ -4660,7 +4660,7 @@
       <c r="I54" s="18"/>
       <c r="J54" s="5"/>
       <c r="M54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N54" t="s">
         <v>50</v>
@@ -4679,7 +4679,7 @@
         <v>36957</v>
       </c>
       <c r="S54" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T54" s="7" t="b">
         <v>1</v>
@@ -4727,7 +4727,7 @@
         <v>36985</v>
       </c>
       <c r="S55" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T55" s="7" t="b">
         <v>1</v>
@@ -4735,7 +4735,7 @@
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="5"/>
@@ -4773,7 +4773,7 @@
         <v>36985</v>
       </c>
       <c r="S56" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T56" s="7" t="b">
         <v>1</v>
@@ -4781,7 +4781,7 @@
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="5"/>
@@ -4792,7 +4792,7 @@
         <v>97</v>
       </c>
       <c r="F57" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>93</v>
@@ -4816,7 +4816,7 @@
         <v>36988</v>
       </c>
       <c r="S57" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T57" s="7" t="b">
         <v>1</v>
@@ -4827,7 +4827,7 @@
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="5"/>
@@ -4838,7 +4838,7 @@
         <v>97</v>
       </c>
       <c r="F58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>98</v>
@@ -4862,7 +4862,7 @@
         <v>36987</v>
       </c>
       <c r="S58" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T58" s="7" t="b">
         <v>1</v>
@@ -4921,7 +4921,7 @@
         <v>36926</v>
       </c>
       <c r="S59" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T59" s="7" t="b">
         <v>1</v>
@@ -4968,7 +4968,7 @@
         <v>36928</v>
       </c>
       <c r="S60" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T60" s="7" t="b">
         <v>1</v>
@@ -4998,7 +4998,7 @@
       <c r="I61" s="18"/>
       <c r="J61" s="5"/>
       <c r="M61" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N61" t="s">
         <v>75</v>
@@ -5017,18 +5017,18 @@
         <v>36986</v>
       </c>
       <c r="S61" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T61" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U61" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="5"/>
@@ -5039,7 +5039,7 @@
         <v>97</v>
       </c>
       <c r="F62" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>93</v>
@@ -5066,7 +5066,7 @@
         <v>36989</v>
       </c>
       <c r="S62" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T62" s="7" t="b">
         <v>1</v>
@@ -5077,7 +5077,7 @@
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="5"/>
@@ -5088,7 +5088,7 @@
         <v>97</v>
       </c>
       <c r="F63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>93</v>
@@ -5114,7 +5114,7 @@
         <v>36989</v>
       </c>
       <c r="S63" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T63" s="7" t="b">
         <v>1</v>
@@ -5166,7 +5166,7 @@
         <v>36927</v>
       </c>
       <c r="S64" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T64" s="7" t="b">
         <v>1</v>
@@ -5174,7 +5174,7 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="5"/>
@@ -5185,7 +5185,7 @@
         <v>97</v>
       </c>
       <c r="F65" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>98</v>
@@ -5196,7 +5196,7 @@
         <v>177</v>
       </c>
       <c r="N65" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O65" s="1" t="s">
         <v>86</v>
@@ -5212,7 +5212,7 @@
         <v>36990</v>
       </c>
       <c r="S65" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T65" s="7" t="b">
         <v>1</v>
@@ -5231,7 +5231,7 @@
         <v>110</v>
       </c>
       <c r="E66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>93</v>
@@ -5239,10 +5239,10 @@
       <c r="I66" s="18"/>
       <c r="J66" s="5"/>
       <c r="M66" t="s">
+        <v>206</v>
+      </c>
+      <c r="N66" t="s">
         <v>207</v>
-      </c>
-      <c r="N66" t="s">
-        <v>208</v>
       </c>
       <c r="O66" s="1" t="s">
         <v>165</v>
@@ -5258,18 +5258,18 @@
         <v>36986</v>
       </c>
       <c r="S66" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T66" s="7" t="b">
         <v>1</v>
       </c>
       <c r="U66" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="5"/>
@@ -5277,7 +5277,7 @@
         <v>111</v>
       </c>
       <c r="E67" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>142</v>
@@ -5285,10 +5285,10 @@
       <c r="I67" s="18"/>
       <c r="J67" s="5"/>
       <c r="M67" t="s">
+        <v>287</v>
+      </c>
+      <c r="N67" t="s">
         <v>288</v>
-      </c>
-      <c r="N67" t="s">
-        <v>289</v>
       </c>
       <c r="O67" s="1" t="s">
         <v>86</v>
@@ -5301,18 +5301,18 @@
         <v>36964</v>
       </c>
       <c r="S67" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T67" s="7" t="b">
         <v>0</v>
       </c>
       <c r="U67" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="5"/>
@@ -5320,7 +5320,7 @@
         <v>110</v>
       </c>
       <c r="E68" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>98</v>
@@ -5328,10 +5328,10 @@
       <c r="I68" s="18"/>
       <c r="J68" s="5"/>
       <c r="M68" t="s">
+        <v>287</v>
+      </c>
+      <c r="N68" t="s">
         <v>288</v>
-      </c>
-      <c r="N68" t="s">
-        <v>289</v>
       </c>
       <c r="O68" s="1" t="s">
         <v>86</v>
@@ -5344,18 +5344,18 @@
         <v>36964</v>
       </c>
       <c r="S68" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T68" s="7" t="b">
         <v>0</v>
       </c>
       <c r="U68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="5"/>
@@ -5363,7 +5363,7 @@
         <v>110</v>
       </c>
       <c r="E69" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>98</v>
@@ -5371,10 +5371,10 @@
       <c r="I69" s="18"/>
       <c r="J69" s="5"/>
       <c r="M69" t="s">
+        <v>287</v>
+      </c>
+      <c r="N69" t="s">
         <v>288</v>
-      </c>
-      <c r="N69" t="s">
-        <v>289</v>
       </c>
       <c r="O69" s="1" t="s">
         <v>86</v>
@@ -5387,7 +5387,7 @@
         <v>36964</v>
       </c>
       <c r="S69" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T69" s="7" t="b">
         <v>0</v>
@@ -5395,7 +5395,7 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="5"/>
@@ -5403,10 +5403,10 @@
         <v>110</v>
       </c>
       <c r="E70" t="s">
+        <v>294</v>
+      </c>
+      <c r="F70" t="s">
         <v>295</v>
-      </c>
-      <c r="F70" t="s">
-        <v>296</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>142</v>
@@ -5414,10 +5414,10 @@
       <c r="I70" s="18"/>
       <c r="J70" s="5"/>
       <c r="M70" t="s">
+        <v>287</v>
+      </c>
+      <c r="N70" t="s">
         <v>288</v>
-      </c>
-      <c r="N70" t="s">
-        <v>289</v>
       </c>
       <c r="O70" s="1" t="s">
         <v>86</v>
@@ -5430,18 +5430,18 @@
         <v>36964</v>
       </c>
       <c r="S70" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T70" s="7" t="b">
         <v>0</v>
       </c>
       <c r="U70" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B71" s="6"/>
       <c r="C71" s="5"/>
@@ -5471,12 +5471,12 @@
       <c r="S71" s="7"/>
       <c r="T71" s="7"/>
       <c r="U71" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="5"/>
@@ -5506,12 +5506,12 @@
       <c r="S72" s="7"/>
       <c r="T72" s="7"/>
       <c r="U72" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="5"/>
@@ -5541,12 +5541,12 @@
       <c r="S73" s="7"/>
       <c r="T73" s="7"/>
       <c r="U73" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="5"/>
@@ -5573,12 +5573,12 @@
       <c r="S74" s="7"/>
       <c r="T74" s="7"/>
       <c r="U74" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="5"/>
@@ -5608,12 +5608,12 @@
       <c r="S75" s="7"/>
       <c r="T75" s="7"/>
       <c r="U75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B76" s="6"/>
       <c r="C76" s="5"/>
@@ -5643,12 +5643,12 @@
       <c r="S76" s="7"/>
       <c r="T76" s="7"/>
       <c r="U76" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="5"/>
@@ -5675,12 +5675,12 @@
       <c r="S77" s="7"/>
       <c r="T77" s="7"/>
       <c r="U77" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="5"/>
@@ -5710,7 +5710,7 @@
       <c r="S78" s="7"/>
       <c r="T78" s="7"/>
       <c r="U78" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
@@ -5919,10 +5919,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D10" s="8">
         <v>36979</v>
@@ -5930,10 +5930,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11" t="s">
         <v>253</v>
-      </c>
-      <c r="B11" t="s">
-        <v>254</v>
       </c>
       <c r="D11" s="8"/>
     </row>
@@ -6636,7 +6636,7 @@
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F32" s="8">
         <v>36990</v>
@@ -6664,7 +6664,7 @@
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F33" s="8">
         <v>36990</v>
@@ -6692,7 +6692,7 @@
         <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F34" s="8">
         <v>36990</v>
@@ -6714,7 +6714,7 @@
         <v>6</v>
       </c>
       <c r="E35" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F35" s="8">
         <v>36990</v>
@@ -6742,7 +6742,7 @@
         <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F36" s="8">
         <v>36990</v>
@@ -6770,7 +6770,7 @@
         <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F37" s="8">
         <v>36990</v>
@@ -6786,10 +6786,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" t="b" cm="1">
@@ -6803,10 +6803,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>246</v>
+      </c>
+      <c r="B39" t="s">
         <v>247</v>
-      </c>
-      <c r="B39" t="s">
-        <v>248</v>
       </c>
       <c r="C39" t="s">
         <v>46</v>
@@ -6815,7 +6815,7 @@
         <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F39" s="8">
         <v>36892</v>
@@ -6831,22 +6831,22 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>280</v>
+      </c>
+      <c r="B40" t="s">
         <v>281</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>282</v>
-      </c>
-      <c r="C40" t="s">
-        <v>283</v>
       </c>
       <c r="D40">
         <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G40" t="b" cm="1">
         <f t="array" ref="G40">AND(POI[[#This Row],[Open Date]]&gt;0, POI[[#This Row],[Open Date]]&lt;=Date[])</f>
@@ -6859,13 +6859,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F41" s="8">
         <v>36892</v>

</xml_diff>

<commit_message>
Crew management + bonuses
</commit_message>
<xml_diff>
--- a/Somewhere Census.xlsx
+++ b/Somewhere Census.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\campaigns\fractured-worlds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0AE7FD-4908-4761-8CF9-C95B37CBB334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E052B20C-EF66-481D-94BC-9BFB787EDF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{206A7769-913C-44FD-A917-4F208E1EA77B}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="312">
   <si>
     <t>Name</t>
   </si>
@@ -998,6 +998,9 @@
   </si>
   <si>
     <t>Deldric Helcral</t>
+  </si>
+  <si>
+    <t>9ish</t>
   </si>
 </sst>
 </file>
@@ -1533,8 +1536,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49AC7A25-6290-4C6E-83CC-C498AF8A8E12}" name="Citizens" displayName="Citizens" ref="A3:U79" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A3:U79" xr:uid="{49AC7A25-6290-4C6E-83CC-C498AF8A8E12}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49AC7A25-6290-4C6E-83CC-C498AF8A8E12}" name="Citizens" displayName="Citizens" ref="A3:U80" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A3:U80" xr:uid="{49AC7A25-6290-4C6E-83CC-C498AF8A8E12}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:U66">
     <sortCondition ref="A3:A66"/>
   </sortState>
@@ -1925,7 +1928,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,14 +1956,14 @@
       </c>
       <c r="B2" s="29">
         <f>B4-B3</f>
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C2" s="30">
         <f>COUNTIF(Citizens[Arrived],FALSE)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G2" s="7">
-        <v>36989</v>
+        <v>37043</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1978,7 +1981,7 @@
       </c>
       <c r="B4" s="29">
         <f>COUNTIF(Citizens[Arrived],TRUE)</f>
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1997,13 +2000,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DF9828-70DC-4E00-A437-C74583D34CC6}">
-  <dimension ref="A1:U79"/>
+  <dimension ref="A1:U80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2191,7 +2194,7 @@
       </c>
       <c r="Q4" s="3" t="b" cm="1">
         <f t="array" ref="Q4">AND(Citizens[[#This Row],[Date of Arrival in Somewhere]]&gt;0, Citizens[[#This Row],[Date of Arrival in Somewhere]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="9">
         <v>36990</v>
@@ -3099,7 +3102,7 @@
       </c>
       <c r="Q22" t="b" cm="1">
         <f t="array" ref="Q22">AND(Citizens[[#This Row],[Date of Arrival in Somewhere]]&gt;0, Citizens[[#This Row],[Date of Arrival in Somewhere]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22" s="7">
         <v>36993</v>
@@ -3192,7 +3195,9 @@
       <c r="N24" t="s">
         <v>47</v>
       </c>
-      <c r="O24" s="1"/>
+      <c r="O24" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="P24">
         <v>1</v>
       </c>
@@ -3531,7 +3536,7 @@
       </c>
       <c r="Q31" t="b" cm="1">
         <f t="array" ref="Q31">AND(Citizens[[#This Row],[Date of Arrival in Somewhere]]&gt;0, Citizens[[#This Row],[Date of Arrival in Somewhere]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" s="7">
         <v>36991</v>
@@ -3629,7 +3634,7 @@
       </c>
       <c r="Q33" t="b" cm="1">
         <f t="array" ref="Q33">AND(Citizens[[#This Row],[Date of Arrival in Somewhere]]&gt;0, Citizens[[#This Row],[Date of Arrival in Somewhere]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33" s="7">
         <v>36993</v>
@@ -4236,7 +4241,7 @@
       </c>
       <c r="Q45" t="b" cm="1">
         <f t="array" ref="Q45">AND(Citizens[[#This Row],[Date of Arrival in Somewhere]]&gt;0, Citizens[[#This Row],[Date of Arrival in Somewhere]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R45" s="7">
         <v>36992</v>
@@ -5206,7 +5211,7 @@
       </c>
       <c r="Q65" t="b" cm="1">
         <f t="array" ref="Q65">AND(Citizens[[#This Row],[Date of Arrival in Somewhere]]&gt;0, Citizens[[#This Row],[Date of Arrival in Somewhere]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R65" s="7">
         <v>36990</v>
@@ -5236,7 +5241,12 @@
       <c r="G66" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I66" s="18"/>
+      <c r="H66" t="s">
+        <v>311</v>
+      </c>
+      <c r="I66" s="18">
+        <v>46013</v>
+      </c>
       <c r="J66" s="5"/>
       <c r="M66" t="s">
         <v>206</v>
@@ -5717,10 +5727,21 @@
       <c r="A79" s="10"/>
       <c r="B79" s="6"/>
       <c r="C79" s="5"/>
-      <c r="G79" s="5"/>
+      <c r="D79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E79" t="s">
+        <v>128</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>142</v>
+      </c>
       <c r="I79" s="18"/>
       <c r="J79" s="5"/>
       <c r="O79" s="1"/>
+      <c r="P79" t="s">
+        <v>25</v>
+      </c>
       <c r="Q79" t="b" cm="1">
         <f t="array" ref="Q79">AND(Citizens[[#This Row],[Date of Arrival in Somewhere]]&gt;0, Citizens[[#This Row],[Date of Arrival in Somewhere]]&lt;=Date[])</f>
         <v>0</v>
@@ -5728,6 +5749,25 @@
       <c r="R79" s="7"/>
       <c r="S79" s="7"/>
       <c r="T79" s="7"/>
+      <c r="U79" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A80" s="10"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="I80" s="18"/>
+      <c r="J80" s="5"/>
+      <c r="O80" s="1"/>
+      <c r="Q80" t="b" cm="1">
+        <f t="array" ref="Q80">AND(Citizens[[#This Row],[Date of Arrival in Somewhere]]&gt;0, Citizens[[#This Row],[Date of Arrival in Somewhere]]&lt;=Date[])</f>
+        <v>0</v>
+      </c>
+      <c r="R80" s="7"/>
+      <c r="S80" s="7"/>
+      <c r="T80" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5736,7 +5776,7 @@
     <mergeCell ref="C1:L1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="N4:N79">
+  <conditionalFormatting sqref="N4:N80">
     <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>AND($G4="Child", $N4="")</formula>
     </cfRule>
@@ -5744,45 +5784,45 @@
       <formula>LEN(TRIM(N4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O79">
+  <conditionalFormatting sqref="O4:O80">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>NOT($O4="y")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q4:Q79">
+  <conditionalFormatting sqref="Q4:Q80">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4:N79" xr:uid="{5E38E75E-415F-4577-90A7-DBDD8840718C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4:N80" xr:uid="{5E38E75E-415F-4577-90A7-DBDD8840718C}">
       <formula1>Businesses</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="P4:P79" xr:uid="{C0D9F438-BAC2-420A-968E-F03BA472BBCE}">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="P4:P80" xr:uid="{C0D9F438-BAC2-420A-968E-F03BA472BBCE}">
       <formula1>Dist</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D79" xr:uid="{5662BE4C-A78C-47B6-B9E3-DFDBAAC7B269}">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D80" xr:uid="{5662BE4C-A78C-47B6-B9E3-DFDBAAC7B269}">
       <formula1>"f, m"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C79" xr:uid="{126FFE62-3B2D-4FE0-8F16-7A2101893CBE}">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C80" xr:uid="{126FFE62-3B2D-4FE0-8F16-7A2101893CBE}">
       <formula1>"LG, NG, CG, LN, N, CN, LE, NE, CE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:J79" xr:uid="{ADF2BB71-101D-46C4-BE4F-145502640A0A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:J80" xr:uid="{ADF2BB71-101D-46C4-BE4F-145502640A0A}">
       <formula1>"very low, low, slightly low, medium, slightly high, high, very high"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:K79" xr:uid="{0D308854-B48C-4E72-B456-1E2329341122}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:K80" xr:uid="{0D308854-B48C-4E72-B456-1E2329341122}">
       <formula1>"very low, low, average, high, very high"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G79" xr:uid="{3F396D49-C608-4436-B5FE-B57097A069F1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G80" xr:uid="{3F396D49-C608-4436-B5FE-B57097A069F1}">
       <formula1>"Child, Young Adult, Adult, Old"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O4:O79" xr:uid="{0DEBB3D4-54EA-4FD0-80AD-E65AD51B7B3F}">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O4:O80" xr:uid="{0DEBB3D4-54EA-4FD0-80AD-E65AD51B7B3F}">
       <formula1>"n,y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S4:S79" xr:uid="{E568529C-5B05-4615-A0A6-89ED936B1FAB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S4:S80" xr:uid="{E568529C-5B05-4615-A0A6-89ED936B1FAB}">
       <formula1>"appeared, migrated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="T4:T79" xr:uid="{77BB72C1-96D2-470F-905B-1CC968FD7BDC}">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="T4:T80" xr:uid="{77BB72C1-96D2-470F-905B-1CC968FD7BDC}">
       <formula1>"FALSE, TRUE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5950,8 +5990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81432F13-4FE0-4020-B411-030E66C8AAC6}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6643,7 +6683,7 @@
       </c>
       <c r="G32" t="b" cm="1">
         <f t="array" ref="G32">AND(POI[[#This Row],[Open Date]]&gt;0, POI[[#This Row],[Open Date]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <f>COUNTIF(Citizens[Workplace],POI[[#This Row],[Name]])</f>
@@ -6671,7 +6711,7 @@
       </c>
       <c r="G33" t="b" cm="1">
         <f t="array" ref="G33">AND(POI[[#This Row],[Open Date]]&gt;0, POI[[#This Row],[Open Date]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
         <f>COUNTIF(Citizens[Workplace],POI[[#This Row],[Name]])</f>
@@ -6699,7 +6739,7 @@
       </c>
       <c r="G34" t="b" cm="1">
         <f t="array" ref="G34">AND(POI[[#This Row],[Open Date]]&gt;0, POI[[#This Row],[Open Date]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
         <f>COUNTIF(Citizens[Workplace],POI[[#This Row],[Name]])</f>
@@ -6721,7 +6761,7 @@
       </c>
       <c r="G35" t="b" cm="1">
         <f t="array" ref="G35">AND(POI[[#This Row],[Open Date]]&gt;0, POI[[#This Row],[Open Date]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <f>COUNTIF(Citizens[Workplace],POI[[#This Row],[Name]])</f>
@@ -6749,7 +6789,7 @@
       </c>
       <c r="G36" t="b" cm="1">
         <f t="array" ref="G36">AND(POI[[#This Row],[Open Date]]&gt;0, POI[[#This Row],[Open Date]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36">
         <f>COUNTIF(Citizens[Workplace],POI[[#This Row],[Name]])</f>
@@ -6777,7 +6817,7 @@
       </c>
       <c r="G37" t="b" cm="1">
         <f t="array" ref="G37">AND(POI[[#This Row],[Open Date]]&gt;0, POI[[#This Row],[Open Date]]&lt;=Date[])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <f>COUNTIF(Citizens[Workplace],POI[[#This Row],[Name]])</f>

</xml_diff>